<commit_message>
Discrepantes - Concluído (Validar em reunião)
</commit_message>
<xml_diff>
--- a/form4/belem_atualizado_form4v2.xlsx
+++ b/form4/belem_atualizado_form4v2.xlsx
@@ -41,7 +41,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'11.25'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'12.25'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'Irregulares'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Discrepantes'!$A$1:$N$24</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -107,7 +106,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="15">
     <fill>
       <patternFill/>
     </fill>
@@ -192,30 +191,6 @@
         <bgColor rgb="00A020F0"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF6400"/>
-        <bgColor rgb="00FF6400"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFC000"/>
-        <bgColor rgb="00FFC000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -281,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -371,24 +346,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="16" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="17" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="18" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3160,19 +3117,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
     <col width="19" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="23" customWidth="1" min="6" max="6"/>
     <col width="29" customWidth="1" min="7" max="7"/>
@@ -3183,6 +3140,8 @@
     <col width="39" customWidth="1" min="12" max="12"/>
     <col width="32" customWidth="1" min="13" max="13"/>
     <col width="26" customWidth="1" min="14" max="14"/>
+    <col width="32" customWidth="1" min="15" max="15"/>
+    <col width="21" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3256,1519 +3215,18 @@
           <t>Renda Média (R$)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B2" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C2" s="32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D2" s="32" t="inlineStr">
-        <is>
-          <t>Thiago da Silva Santos</t>
-        </is>
-      </c>
-      <c r="E2" s="32" t="inlineStr">
-        <is>
-          <t>06.25</t>
-        </is>
-      </c>
-      <c r="F2" s="32" t="inlineStr">
-        <is>
-          <t>09/07/2025</t>
-        </is>
-      </c>
-      <c r="G2" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H2" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="34" t="n">
-        <v>1056.2</v>
-      </c>
-      <c r="J2" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K2" s="33" t="n">
-        <v>5.46</v>
-      </c>
-      <c r="L2" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M2" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N2" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B3" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C3" s="32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D3" s="32" t="inlineStr">
-        <is>
-          <t>Thiago da Silva Santos</t>
-        </is>
-      </c>
-      <c r="E3" s="32" t="inlineStr">
-        <is>
-          <t>05.25</t>
-        </is>
-      </c>
-      <c r="F3" s="32" t="inlineStr">
-        <is>
-          <t>06/06/2025</t>
-        </is>
-      </c>
-      <c r="G3" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J3" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K3" s="33" t="n">
-        <v>7.43</v>
-      </c>
-      <c r="L3" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M3" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N3" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B4" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C4" s="32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D4" s="32" t="inlineStr">
-        <is>
-          <t>Thiago da Silva Santos</t>
-        </is>
-      </c>
-      <c r="E4" s="32" t="inlineStr">
-        <is>
-          <t>04.25</t>
-        </is>
-      </c>
-      <c r="F4" s="32" t="inlineStr">
-        <is>
-          <t>09/05/2025</t>
-        </is>
-      </c>
-      <c r="G4" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H4" s="33" t="n">
-        <v>2232.5</v>
-      </c>
-      <c r="I4" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J4" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K4" s="33" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="L4" s="34" t="n">
-        <v>64.7715</v>
-      </c>
-      <c r="M4" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N4" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B5" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C5" s="32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D5" s="32" t="inlineStr">
-        <is>
-          <t>Thiago da Silva Santos</t>
-        </is>
-      </c>
-      <c r="E5" s="32" t="inlineStr">
-        <is>
-          <t>03.25</t>
-        </is>
-      </c>
-      <c r="F5" s="32" t="inlineStr">
-        <is>
-          <t>09/04/2025</t>
-        </is>
-      </c>
-      <c r="G5" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H5" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J5" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K5" s="33" t="n">
-        <v>8.449999999999999</v>
-      </c>
-      <c r="L5" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M5" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N5" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B6" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C6" s="32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D6" s="32" t="inlineStr">
-        <is>
-          <t>Thiago da Silva Santos</t>
-        </is>
-      </c>
-      <c r="E6" s="32" t="inlineStr">
-        <is>
-          <t>02.25</t>
-        </is>
-      </c>
-      <c r="F6" s="32" t="inlineStr">
-        <is>
-          <t>07/03/2025</t>
-        </is>
-      </c>
-      <c r="G6" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H6" s="33" t="n">
-        <v>32596.43</v>
-      </c>
-      <c r="I6" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="33" t="n">
-        <v>11.85</v>
-      </c>
-      <c r="L6" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M6" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N6" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B7" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C7" s="32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D7" s="32" t="inlineStr">
-        <is>
-          <t>Thiago da Silva Santos</t>
-        </is>
-      </c>
-      <c r="E7" s="32" t="inlineStr">
-        <is>
-          <t>01.25</t>
-        </is>
-      </c>
-      <c r="F7" s="32" t="inlineStr">
-        <is>
-          <t>12/03/2025</t>
-        </is>
-      </c>
-      <c r="G7" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H7" s="33" t="n">
-        <v>32596.43</v>
-      </c>
-      <c r="I7" s="34" t="n">
-        <v>2985.52</v>
-      </c>
-      <c r="J7" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K7" s="33" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="L7" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M7" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N7" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B8" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C8" s="32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D8" s="32" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
-      </c>
-      <c r="E8" s="32" t="inlineStr">
-        <is>
-          <t>05.25</t>
-        </is>
-      </c>
-      <c r="F8" s="32" t="inlineStr">
-        <is>
-          <t>12/06/2025</t>
-        </is>
-      </c>
-      <c r="G8" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H8" s="34" t="n">
-        <v>11363</v>
-      </c>
-      <c r="I8" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J8" s="34" t="n">
-        <v>26.21</v>
-      </c>
-      <c r="K8" s="34" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="L8" s="34" t="n">
-        <v>27.94</v>
-      </c>
-      <c r="M8" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N8" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B9" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C9" s="32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D9" s="32" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
-      </c>
-      <c r="E9" s="32" t="inlineStr">
-        <is>
-          <t>04.25</t>
-        </is>
-      </c>
-      <c r="F9" s="32" t="inlineStr">
-        <is>
-          <t>10/05/2025</t>
-        </is>
-      </c>
-      <c r="G9" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H9" s="33" t="n">
-        <v>19770</v>
-      </c>
-      <c r="I9" s="33" t="n">
-        <v>21875.55</v>
-      </c>
-      <c r="J9" s="33" t="n">
-        <v>34.54</v>
-      </c>
-      <c r="K9" s="35" t="n">
-        <v>1.83</v>
-      </c>
-      <c r="L9" s="33" t="n">
-        <v>36.37</v>
-      </c>
-      <c r="M9" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N9" s="34" t="n">
-        <v>1862.41</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B10" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C10" s="32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D10" s="32" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
-      </c>
-      <c r="E10" s="32" t="inlineStr">
-        <is>
-          <t>03.25</t>
-        </is>
-      </c>
-      <c r="F10" s="32" t="inlineStr">
-        <is>
-          <t>15/04/2025</t>
-        </is>
-      </c>
-      <c r="G10" s="34" t="n">
-        <v>32714.25</v>
-      </c>
-      <c r="H10" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="34" t="n">
-        <v>11862.61</v>
-      </c>
-      <c r="J10" s="33" t="n">
-        <v>45.42</v>
-      </c>
-      <c r="K10" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="33" t="n">
-        <v>46.62</v>
-      </c>
-      <c r="M10" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N10" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B11" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C11" s="32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D11" s="32" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
-      </c>
-      <c r="E11" s="32" t="inlineStr">
-        <is>
-          <t>02.25</t>
-        </is>
-      </c>
-      <c r="F11" s="32" t="inlineStr">
-        <is>
-          <t>09/04/2025</t>
-        </is>
-      </c>
-      <c r="G11" s="34" t="n">
-        <v>32408</v>
-      </c>
-      <c r="H11" s="35" t="n">
-        <v>3133.12</v>
-      </c>
-      <c r="I11" s="33" t="n">
-        <v>18453.14</v>
-      </c>
-      <c r="J11" s="33" t="n">
-        <v>45.15</v>
-      </c>
-      <c r="K11" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L11" s="33" t="n">
-        <v>46.45</v>
-      </c>
-      <c r="M11" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N11" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B12" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C12" s="32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D12" s="32" t="inlineStr">
-        <is>
-          <t>Jackson Souza Soeiro</t>
-        </is>
-      </c>
-      <c r="E12" s="32" t="inlineStr">
-        <is>
-          <t>01.25</t>
-        </is>
-      </c>
-      <c r="F12" s="32" t="inlineStr">
-        <is>
-          <t>24/02/2025</t>
-        </is>
-      </c>
-      <c r="G12" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H12" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I12" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J12" s="35" t="n">
-        <v>3.71971</v>
-      </c>
-      <c r="K12" s="35" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L12" s="35" t="n">
-        <v>4.14551</v>
-      </c>
-      <c r="M12" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N12" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B13" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C13" s="32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D13" s="32" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E13" s="32" t="inlineStr">
-        <is>
-          <t>06.25</t>
-        </is>
-      </c>
-      <c r="F13" s="32" t="inlineStr">
-        <is>
-          <t>13/07/2025</t>
-        </is>
-      </c>
-      <c r="G13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I13" s="33" t="n">
-        <v>33088</v>
-      </c>
-      <c r="J13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K13" s="33" t="n">
-        <v>5.95</v>
-      </c>
-      <c r="L13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B14" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C14" s="32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D14" s="32" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E14" s="32" t="inlineStr">
-        <is>
-          <t>05.25</t>
-        </is>
-      </c>
-      <c r="F14" s="32" t="inlineStr">
-        <is>
-          <t>10/06/2025</t>
-        </is>
-      </c>
-      <c r="G14" s="35" t="n">
-        <v>10175</v>
-      </c>
-      <c r="H14" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I14" s="33" t="n">
-        <v>33649</v>
-      </c>
-      <c r="J14" s="35" t="n">
-        <v>22.32</v>
-      </c>
-      <c r="K14" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L14" s="34" t="n">
-        <v>23.96</v>
-      </c>
-      <c r="M14" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N14" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B15" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C15" s="32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D15" s="32" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E15" s="32" t="inlineStr">
-        <is>
-          <t>04.25</t>
-        </is>
-      </c>
-      <c r="F15" s="32" t="inlineStr">
-        <is>
-          <t>10/05/2025</t>
-        </is>
-      </c>
-      <c r="G15" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H15" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I15" s="33" t="n">
-        <v>29754.4</v>
-      </c>
-      <c r="J15" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K15" s="33" t="n">
-        <v>4.94</v>
-      </c>
-      <c r="L15" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M15" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N15" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B16" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C16" s="32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D16" s="32" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E16" s="32" t="inlineStr">
-        <is>
-          <t>03.25</t>
-        </is>
-      </c>
-      <c r="F16" s="32" t="inlineStr">
-        <is>
-          <t>09/04/2025</t>
-        </is>
-      </c>
-      <c r="G16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I16" s="33" t="n">
-        <v>32751.9</v>
-      </c>
-      <c r="J16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N16" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B17" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C17" s="32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D17" s="32" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E17" s="32" t="inlineStr">
-        <is>
-          <t>02.25</t>
-        </is>
-      </c>
-      <c r="F17" s="32" t="inlineStr">
-        <is>
-          <t>06/03/2025</t>
-        </is>
-      </c>
-      <c r="G17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M17" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N17" s="34" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B18" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C18" s="32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D18" s="32" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E18" s="32" t="inlineStr">
-        <is>
-          <t>01.25</t>
-        </is>
-      </c>
-      <c r="F18" s="32" t="inlineStr">
-        <is>
-          <t>12/02/2025</t>
-        </is>
-      </c>
-      <c r="G18" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H18" s="33" t="n">
-        <v>1500</v>
-      </c>
-      <c r="I18" s="33" t="n">
-        <v>34581.31</v>
-      </c>
-      <c r="J18" s="36" t="n">
-        <v>59758</v>
-      </c>
-      <c r="K18" s="33" t="n">
-        <v>9</v>
-      </c>
-      <c r="L18" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M18" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N18" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B19" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C19" s="32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D19" s="32" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E19" s="32" t="inlineStr">
-        <is>
-          <t>06.25</t>
-        </is>
-      </c>
-      <c r="F19" s="32" t="inlineStr">
-        <is>
-          <t>11/07/2025</t>
-        </is>
-      </c>
-      <c r="G19" s="33" t="n">
-        <v>91384.87</v>
-      </c>
-      <c r="H19" s="34" t="n">
-        <v>12792.86</v>
-      </c>
-      <c r="I19" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J19" s="33" t="n">
-        <v>121.5419</v>
-      </c>
-      <c r="K19" s="33" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="L19" s="33" t="n">
-        <v>123.6619</v>
-      </c>
-      <c r="M19" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N19" s="33" t="n">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B20" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C20" s="32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D20" s="32" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E20" s="32" t="inlineStr">
-        <is>
-          <t>05.25</t>
-        </is>
-      </c>
-      <c r="F20" s="32" t="inlineStr">
-        <is>
-          <t>18/06/2025</t>
-        </is>
-      </c>
-      <c r="G20" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H20" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I20" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J20" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K20" s="33" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="L20" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M20" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N20" s="33" t="n">
-        <v>1262.36</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B21" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C21" s="32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D21" s="32" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E21" s="32" t="inlineStr">
-        <is>
-          <t>04.25</t>
-        </is>
-      </c>
-      <c r="F21" s="32" t="inlineStr">
-        <is>
-          <t>12/05/2025</t>
-        </is>
-      </c>
-      <c r="G21" s="34" t="n">
-        <v>14750.41</v>
-      </c>
-      <c r="H21" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J21" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K21" s="33" t="n">
-        <v>3.17</v>
-      </c>
-      <c r="L21" s="34" t="n">
-        <v>25.48</v>
-      </c>
-      <c r="M21" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N21" s="33" t="n">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B22" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C22" s="32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D22" s="32" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E22" s="32" t="inlineStr">
-        <is>
-          <t>03.25</t>
-        </is>
-      </c>
-      <c r="F22" s="32" t="inlineStr">
-        <is>
-          <t>10/04/2025</t>
-        </is>
-      </c>
-      <c r="G22" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H22" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I22" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J22" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K22" s="33" t="n">
-        <v>2.51</v>
-      </c>
-      <c r="L22" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M22" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N22" s="33" t="n">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B23" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C23" s="32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D23" s="32" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E23" s="32" t="inlineStr">
-        <is>
-          <t>02.25</t>
-        </is>
-      </c>
-      <c r="F23" s="32" t="inlineStr">
-        <is>
-          <t>24/03/2025</t>
-        </is>
-      </c>
-      <c r="G23" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H23" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I23" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J23" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K23" s="35" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="L23" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M23" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N23" s="33" t="n">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="32" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B24" s="32" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C24" s="32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D24" s="32" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E24" s="32" t="inlineStr">
-        <is>
-          <t>01.25</t>
-        </is>
-      </c>
-      <c r="F24" s="32" t="inlineStr">
-        <is>
-          <t>13/02/2025</t>
-        </is>
-      </c>
-      <c r="G24" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H24" s="35" t="n">
-        <v>44607</v>
-      </c>
-      <c r="I24" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J24" s="36" t="n">
-        <v>18961</v>
-      </c>
-      <c r="K24" s="33" t="n">
-        <v>3.81</v>
-      </c>
-      <c r="L24" s="36" t="n">
-        <v>22769</v>
-      </c>
-      <c r="M24" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N24" s="33" t="n">
-        <v>1200</v>
+      <c r="O1" s="24" t="inlineStr">
+        <is>
+          <t>Validado pelo Regional</t>
+        </is>
+      </c>
+      <c r="P1" s="24" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N24"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7187,12 +5645,16 @@
         <f>IFERROR(IF(INDEX('01.25'!D2:D500, MATCH(B4&amp;C4, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))="", "", INDEX('01.25'!D2:D500, MATCH(B4&amp;C4, INDEX('01.25'!B2:B500&amp;'01.25'!C2:C500, 0), 0))), "")</f>
         <v/>
       </c>
-      <c r="E4" s="31" t="inlineStr">
-        <is>
-          <t>Atrasado</t>
-        </is>
-      </c>
-      <c r="F4" s="26" t="n"/>
+      <c r="E4" s="27" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F4" s="26" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
       <c r="G4" s="29" t="inlineStr">
         <is>
           <t>Não</t>

</xml_diff>

<commit_message>
estilização da coluna dos regionais - discrepantes
</commit_message>
<xml_diff>
--- a/form4/belem_atualizado_form4v2.xlsx
+++ b/form4/belem_atualizado_form4v2.xlsx
@@ -4323,10 +4323,14 @@
         </is>
       </c>
       <c r="H3" s="26" t="n"/>
-      <c r="I3" s="26" t="n"/>
+      <c r="I3" s="26" t="inlineStr">
+        <is>
+          <t>Deletar 4308</t>
+        </is>
+      </c>
       <c r="J3" s="26" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Em Análise</t>
         </is>
       </c>
       <c r="K3" s="26" t="n"/>

</xml_diff>